<commit_message>
Added more static data to Project_Report.xlsx (till 11-20-2020).
</commit_message>
<xml_diff>
--- a/power-bi-reports/Project_Report.xlsx
+++ b/power-bi-reports/Project_Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\dan\azure\spotlight\PowerBI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\dan\azure\current\license-server\power-bi-reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18563" windowHeight="7928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18563" windowHeight="9188" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Summary" sheetId="2" r:id="rId1"/>
@@ -482,19 +482,19 @@
       </c>
       <c r="D2" s="1">
         <f>SUM('Ctaas Summary'!B2:'Ctaas Summary'!B24)</f>
-        <v>400</v>
+        <v>460</v>
       </c>
       <c r="E2" s="1">
         <f>SUM('Ctaas Summary'!C2:'Ctaas Summary'!C24)</f>
-        <v>216</v>
+        <v>249</v>
       </c>
       <c r="F2" s="1">
         <f>SUM('Ctaas Summary'!D2:'Ctaas Summary'!D24)</f>
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="G2" s="1">
         <f>F2/D2*100</f>
-        <v>46</v>
+        <v>45.869565217391305</v>
       </c>
     </row>
   </sheetData>
@@ -504,10 +504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1208,6 +1208,633 @@
         <v>1</v>
       </c>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="5">
+        <v>44867</v>
+      </c>
+      <c r="B22" s="2">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" ref="E22" si="10">D22/B22*100</f>
+        <v>45</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3</v>
+      </c>
+      <c r="H22" s="2">
+        <v>3</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="5">
+        <v>44868</v>
+      </c>
+      <c r="B23" s="2">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" ref="E23:E40" si="11">D23/B23*100</f>
+        <v>45</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="5">
+        <v>44869</v>
+      </c>
+      <c r="B24" s="2">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>3</v>
+      </c>
+      <c r="H24" s="2">
+        <v>3</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="5">
+        <v>44870</v>
+      </c>
+      <c r="B25" s="2">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2">
+        <v>11</v>
+      </c>
+      <c r="D25" s="2">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3</v>
+      </c>
+      <c r="H25" s="2">
+        <v>3</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="5">
+        <v>44871</v>
+      </c>
+      <c r="B26" s="2">
+        <v>20</v>
+      </c>
+      <c r="C26" s="2">
+        <v>11</v>
+      </c>
+      <c r="D26" s="2">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <v>3</v>
+      </c>
+      <c r="H26" s="2">
+        <v>3</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="5">
+        <v>44872</v>
+      </c>
+      <c r="B27" s="2">
+        <v>20</v>
+      </c>
+      <c r="C27" s="2">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>3</v>
+      </c>
+      <c r="H27" s="2">
+        <v>3</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="5">
+        <v>44873</v>
+      </c>
+      <c r="B28" s="2">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2">
+        <v>11</v>
+      </c>
+      <c r="D28" s="2">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3</v>
+      </c>
+      <c r="H28" s="2">
+        <v>3</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="5">
+        <v>44874</v>
+      </c>
+      <c r="B29" s="2">
+        <v>20</v>
+      </c>
+      <c r="C29" s="2">
+        <v>11</v>
+      </c>
+      <c r="D29" s="2">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3</v>
+      </c>
+      <c r="H29" s="2">
+        <v>3</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="5">
+        <v>44875</v>
+      </c>
+      <c r="B30" s="2">
+        <v>20</v>
+      </c>
+      <c r="C30" s="2">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <v>3</v>
+      </c>
+      <c r="H30" s="2">
+        <v>3</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" s="5">
+        <v>44876</v>
+      </c>
+      <c r="B31" s="2">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2">
+        <v>3</v>
+      </c>
+      <c r="H31" s="2">
+        <v>3</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="5">
+        <v>44877</v>
+      </c>
+      <c r="B32" s="2">
+        <v>20</v>
+      </c>
+      <c r="C32" s="2">
+        <v>11</v>
+      </c>
+      <c r="D32" s="2">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3</v>
+      </c>
+      <c r="H32" s="2">
+        <v>3</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" s="5">
+        <v>44878</v>
+      </c>
+      <c r="B33" s="2">
+        <v>20</v>
+      </c>
+      <c r="C33" s="2">
+        <v>11</v>
+      </c>
+      <c r="D33" s="2">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>3</v>
+      </c>
+      <c r="H33" s="2">
+        <v>3</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" s="5">
+        <v>44879</v>
+      </c>
+      <c r="B34" s="2">
+        <v>20</v>
+      </c>
+      <c r="C34" s="2">
+        <v>11</v>
+      </c>
+      <c r="D34" s="2">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3</v>
+      </c>
+      <c r="H34" s="2">
+        <v>3</v>
+      </c>
+      <c r="I34" s="2">
+        <v>1</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" s="5">
+        <v>44880</v>
+      </c>
+      <c r="B35" s="2">
+        <v>20</v>
+      </c>
+      <c r="C35" s="2">
+        <v>11</v>
+      </c>
+      <c r="D35" s="2">
+        <v>9</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2">
+        <v>3</v>
+      </c>
+      <c r="H35" s="2">
+        <v>3</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" s="5">
+        <v>44881</v>
+      </c>
+      <c r="B36" s="2">
+        <v>20</v>
+      </c>
+      <c r="C36" s="2">
+        <v>11</v>
+      </c>
+      <c r="D36" s="2">
+        <v>9</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2">
+        <v>3</v>
+      </c>
+      <c r="H36" s="2">
+        <v>3</v>
+      </c>
+      <c r="I36" s="2">
+        <v>1</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" s="5">
+        <v>44882</v>
+      </c>
+      <c r="B37" s="2">
+        <v>20</v>
+      </c>
+      <c r="C37" s="2">
+        <v>11</v>
+      </c>
+      <c r="D37" s="2">
+        <v>9</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="2">
+        <v>3</v>
+      </c>
+      <c r="H37" s="2">
+        <v>3</v>
+      </c>
+      <c r="I37" s="2">
+        <v>1</v>
+      </c>
+      <c r="J37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="5">
+        <v>44883</v>
+      </c>
+      <c r="B38" s="2">
+        <v>20</v>
+      </c>
+      <c r="C38" s="2">
+        <v>11</v>
+      </c>
+      <c r="D38" s="2">
+        <v>9</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2">
+        <v>3</v>
+      </c>
+      <c r="H38" s="2">
+        <v>3</v>
+      </c>
+      <c r="I38" s="2">
+        <v>1</v>
+      </c>
+      <c r="J38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B39" s="2">
+        <v>20</v>
+      </c>
+      <c r="C39" s="2">
+        <v>11</v>
+      </c>
+      <c r="D39" s="2">
+        <v>9</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2">
+        <v>3</v>
+      </c>
+      <c r="H39" s="2">
+        <v>3</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A40" s="5">
+        <v>44885</v>
+      </c>
+      <c r="B40" s="2">
+        <v>20</v>
+      </c>
+      <c r="C40" s="2">
+        <v>11</v>
+      </c>
+      <c r="D40" s="2">
+        <v>9</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3</v>
+      </c>
+      <c r="H40" s="2">
+        <v>3</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1</v>
+      </c>
+      <c r="J40" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>